<commit_message>
Revisión corrector de estilo y final del editor CN_06_08_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/SolicitudGrafica_CN_06_08_CO_REC30.xlsx
+++ b/fuentes/contenidos/grado06/guion08/SolicitudGrafica_CN_06_08_CO_REC30.xlsx
@@ -1560,6 +1560,9 @@
     <xf numFmtId="1" fontId="22" fillId="0" borderId="5" xfId="51" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1657,9 +1660,6 @@
     </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="52">
@@ -2508,8 +2508,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2547,14 +2547,14 @@
       <c r="B2" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="95" t="s">
+      <c r="C2" s="96" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="96"/>
-      <c r="F2" s="88" t="s">
+      <c r="D2" s="97"/>
+      <c r="F2" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="89"/>
+      <c r="G2" s="90"/>
       <c r="H2" s="46"/>
       <c r="I2" s="46"/>
       <c r="J2" s="16"/>
@@ -2564,14 +2564,14 @@
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="97">
+      <c r="C3" s="98">
         <v>6</v>
       </c>
-      <c r="D3" s="98"/>
-      <c r="F3" s="90">
+      <c r="D3" s="99"/>
+      <c r="F3" s="91">
         <v>42119</v>
       </c>
-      <c r="G3" s="91"/>
+      <c r="G3" s="92"/>
       <c r="H3" s="46"/>
       <c r="I3" s="46"/>
       <c r="J3" s="16"/>
@@ -2581,10 +2581,10 @@
       <c r="B4" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="99" t="s">
+      <c r="C4" s="100" t="s">
         <v>148</v>
       </c>
-      <c r="D4" s="100"/>
+      <c r="D4" s="101"/>
       <c r="E4" s="5"/>
       <c r="F4" s="45" t="s">
         <v>55</v>
@@ -2602,10 +2602,10 @@
       <c r="B5" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="101" t="s">
+      <c r="C5" s="102" t="s">
         <v>147</v>
       </c>
-      <c r="D5" s="102"/>
+      <c r="D5" s="103"/>
       <c r="E5" s="5"/>
       <c r="F5" s="43" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2656,12 +2656,12 @@
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="92" t="s">
+      <c r="F8" s="93" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="93"/>
-      <c r="H8" s="93"/>
-      <c r="I8" s="94"/>
+      <c r="G8" s="94"/>
+      <c r="H8" s="94"/>
+      <c r="I8" s="95"/>
       <c r="J8" s="18"/>
       <c r="K8" s="12"/>
       <c r="L8" s="2"/>
@@ -2757,7 +2757,7 @@
         <v>146</v>
       </c>
       <c r="F11" s="14" t="str">
-        <f t="shared" ref="F11:F74" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F11:F16" si="0">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CN_06_08_CO_REC30_F02.jpg</v>
       </c>
       <c r="G11" s="14" t="str">
@@ -2765,7 +2765,7 @@
         <v>950 x 608 px</v>
       </c>
       <c r="H11" s="14" t="str">
-        <f t="shared" ref="H11:H74" si="1">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H11:H16" si="1">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I11" s="14" t="str">
@@ -2779,7 +2779,7 @@
       <c r="A12" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="121" t="s">
+      <c r="B12" s="88" t="s">
         <v>158</v>
       </c>
       <c r="C12" s="72" t="s">
@@ -2851,8 +2851,8 @@
       <c r="A14" s="13" t="s">
         <v>153</v>
       </c>
-      <c r="B14" s="73" t="s">
-        <v>159</v>
+      <c r="B14" s="84" t="s">
+        <v>160</v>
       </c>
       <c r="C14" s="72" t="s">
         <v>162</v>
@@ -2864,19 +2864,19 @@
         <v>146</v>
       </c>
       <c r="F14" s="14" t="str">
-        <f t="shared" si="0"/>
-        <v>CN_06_08_CO_REC30_F05.jpg</v>
+        <f>IF(OR(B17&lt;&gt;"",J14&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I14="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <v/>
       </c>
       <c r="G14" s="14" t="str">
         <f>IF(F14&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>950 x 608 px</v>
+        <v/>
       </c>
       <c r="H14" s="14" t="str">
-        <f t="shared" si="1"/>
+        <f>IF(AND(I14&lt;&gt;"",I14&lt;&gt;0),IF(OR(B17&lt;&gt;"",J14&lt;&gt;""),CONCATENATE($C$7,"_",$A14,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I14" s="14" t="str">
-        <f>IF(OR(B14&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
+        <f>IF(OR(B17&lt;&gt;"",J14&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v/>
       </c>
       <c r="J14" s="75"/>
@@ -2886,8 +2886,8 @@
       <c r="A15" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B15" s="84" t="s">
-        <v>160</v>
+      <c r="B15" s="73" t="s">
+        <v>159</v>
       </c>
       <c r="C15" s="72" t="s">
         <v>162</v>
@@ -2956,7 +2956,7 @@
     </row>
     <row r="17" spans="1:11" s="12" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="13"/>
-      <c r="B17" s="84"/>
+      <c r="B17" s="73"/>
       <c r="C17" s="72"/>
       <c r="D17" s="72"/>
       <c r="E17" s="72"/>
@@ -4061,18 +4061,18 @@
     </row>
     <row r="102" spans="1:11" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A102" s="13" t="str">
-        <f t="shared" ref="A84:A108" si="2">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE(LEFT(A101,3),IF(MID(A101,4,2)+1&lt;10,CONCATENATE("0",MID(A101,4,2)+1),MID(A101,4,2)+1)),"")</f>
+        <f t="shared" ref="A102:A108" si="2">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE(LEFT(A101,3),IF(MID(A101,4,2)+1&lt;10,CONCATENATE("0",MID(A101,4,2)+1),MID(A101,4,2)+1)),"")</f>
         <v/>
       </c>
       <c r="B102" s="13"/>
       <c r="C102" s="25" t="str">
-        <f t="shared" ref="C75:C108" si="3">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C102:C108" si="3">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D102" s="14"/>
       <c r="E102" s="14"/>
       <c r="F102" s="14" t="str">
-        <f t="shared" ref="F75:F108" si="4">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE($C$7,"_",$A102,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I102="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F102:F108" si="4">IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE($C$7,"_",$A102,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I102="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G102" s="14" t="str">
@@ -4080,7 +4080,7 @@
         <v/>
       </c>
       <c r="H102" s="14" t="str">
-        <f t="shared" ref="H75:H108" si="5">IF(AND(I102&lt;&gt;"",I102&lt;&gt;0),IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE($C$7,"_",$A102,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H102:H108" si="5">IF(AND(I102&lt;&gt;"",I102&lt;&gt;0),IF(OR(B102&lt;&gt;"",J102&lt;&gt;""),CONCATENATE($C$7,"_",$A102,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I102" s="14" t="str">
@@ -4327,7 +4327,7 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B15" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId2"/>
@@ -4360,25 +4360,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="106" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="106"/>
-      <c r="D1" s="106"/>
-      <c r="E1" s="106"/>
-      <c r="F1" s="107"/>
+      <c r="B1" s="107"/>
+      <c r="C1" s="107"/>
+      <c r="D1" s="107"/>
+      <c r="E1" s="107"/>
+      <c r="F1" s="108"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="37"/>
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="109" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="109"/>
-      <c r="E2" s="110"/>
+      <c r="D2" s="110"/>
+      <c r="E2" s="111"/>
       <c r="F2" s="38"/>
     </row>
     <row r="3" spans="1:11" ht="63" x14ac:dyDescent="0.25">
@@ -4386,11 +4386,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="37"/>
-      <c r="C3" s="114" t="s">
+      <c r="C3" s="115" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="115"/>
-      <c r="E3" s="116"/>
+      <c r="D3" s="116"/>
+      <c r="E3" s="117"/>
       <c r="F3" s="38"/>
       <c r="H3" s="28" t="s">
         <v>18</v>
@@ -4441,11 +4441,11 @@
       <c r="C5" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="117" t="str">
+      <c r="D5" s="118" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="118"/>
+      <c r="E5" s="119"/>
       <c r="F5" s="38"/>
       <c r="H5" s="28" t="s">
         <v>22</v>
@@ -4490,12 +4490,12 @@
       <c r="C7" s="68" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="103" t="str">
+      <c r="D7" s="104" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="103"/>
-      <c r="F7" s="104"/>
+      <c r="E7" s="104"/>
+      <c r="F7" s="105"/>
       <c r="H7" s="28" t="s">
         <v>24</v>
       </c>
@@ -4589,14 +4589,14 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="105" t="s">
+      <c r="A13" s="106" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="106"/>
-      <c r="C13" s="106"/>
-      <c r="D13" s="106"/>
-      <c r="E13" s="106"/>
-      <c r="F13" s="107"/>
+      <c r="B13" s="107"/>
+      <c r="C13" s="107"/>
+      <c r="D13" s="107"/>
+      <c r="E13" s="107"/>
+      <c r="F13" s="108"/>
       <c r="I13" s="28" t="s">
         <v>33</v>
       </c>
@@ -4629,12 +4629,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="37"/>
-      <c r="C15" s="108" t="s">
+      <c r="C15" s="109" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="109"/>
-      <c r="E15" s="109"/>
-      <c r="F15" s="110"/>
+      <c r="D15" s="110"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="111"/>
       <c r="J15" s="28">
         <v>12</v>
       </c>
@@ -4674,12 +4674,12 @@
       <c r="C17" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="111" t="str">
+      <c r="D17" s="112" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="112"/>
-      <c r="F17" s="113"/>
+      <c r="E17" s="113"/>
+      <c r="F17" s="114"/>
       <c r="J17" s="28">
         <v>14</v>
       </c>
@@ -4695,12 +4695,12 @@
       <c r="C18" s="68" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="103" t="str">
+      <c r="D18" s="104" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="103"/>
-      <c r="F18" s="104"/>
+      <c r="E18" s="104"/>
+      <c r="F18" s="105"/>
       <c r="J18" s="28">
         <v>15</v>
       </c>
@@ -5097,41 +5097,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="119" t="s">
+      <c r="A1" s="120" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="120" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="119" t="s">
+      <c r="C1" s="120" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="119" t="s">
+      <c r="D1" s="120" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="119" t="s">
+      <c r="E1" s="120" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="119" t="s">
+      <c r="F1" s="120" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="119" t="s">
+      <c r="G1" s="120" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="120" t="s">
+      <c r="H1" s="121" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="120"/>
-      <c r="J1" s="120"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="119"/>
-      <c r="B2" s="119"/>
-      <c r="C2" s="119"/>
-      <c r="D2" s="119"/>
-      <c r="E2" s="119"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="119"/>
+      <c r="A2" s="120"/>
+      <c r="B2" s="120"/>
+      <c r="C2" s="120"/>
+      <c r="D2" s="120"/>
+      <c r="E2" s="120"/>
+      <c r="F2" s="120"/>
+      <c r="G2" s="120"/>
       <c r="H2" s="47" t="s">
         <v>65</v>
       </c>

</xml_diff>